<commit_message>
first commit or updating data tables
</commit_message>
<xml_diff>
--- a/processed/germ_tray.xlsx
+++ b/processed/germ_tray.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Library/CloudStorage/Dropbox/GRADSCHOOL/Dissertation/R_dissertation/chaparraldegradation_2022b/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D5CBCE13-3121-CD4A-8B50-D77382E2517D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{720D54DA-A39B-9E47-A1FE-F8EDDC7DE200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="2"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PIVOT" sheetId="3" r:id="rId1"/>
@@ -18,15 +18,28 @@
     <sheet name="x_nativshrubecover" sheetId="2" r:id="rId3"/>
     <sheet name="x_nngrasscover" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="5" r:id="rId5"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="319">
   <si>
     <t>stand_core_depth_treat</t>
   </si>
@@ -980,6 +993,9 @@
   </si>
   <si>
     <t>Count of seeds_per_g_log</t>
+  </si>
+  <si>
+    <t>V4m!WR378s32gDu</t>
   </si>
 </sst>
 </file>
@@ -20094,7 +20110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+    <sheetView topLeftCell="A169" workbookViewId="0">
       <selection activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
@@ -21756,10 +21772,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B206"/>
+  <dimension ref="A1:E206"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="E188" sqref="E188"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23300,7 +23316,7 @@
         <v>-3.83911623462006</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>0.12195122</v>
       </c>
@@ -23308,7 +23324,7 @@
         <v>-4.3091198638657904</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>0.12195122</v>
       </c>
@@ -23316,7 +23332,7 @@
         <v>-3.6159726833058499</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>0.12195122</v>
       </c>
@@ -23324,7 +23340,7 @@
         <v>-3.0208059111061099</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>0.12195122</v>
       </c>
@@ -23332,7 +23348,7 @@
         <v>-2.7976623597919001</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>0.12195122</v>
       </c>
@@ -23340,15 +23356,18 @@
         <v>-3.4908095403518402</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>0.12195122</v>
       </c>
       <c r="B198">
         <v>-2.1045151792319499</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E198" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>0.12195122</v>
       </c>
@@ -23356,7 +23375,7 @@
         <v>-4.5322634151800001</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>0.12195122</v>
       </c>
@@ -23364,7 +23383,7 @@
         <v>-4.81994548763178</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>0.12195122</v>
       </c>
@@ -23372,7 +23391,7 @@
         <v>-4.3091198638657904</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>0.12195122</v>
       </c>
@@ -23380,7 +23399,7 @@
         <v>-3.27950044668464</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>0.12195122</v>
       </c>
@@ -23388,7 +23407,7 @@
         <v>-2.2098756948897802</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>0.12195122</v>
       </c>
@@ -23396,7 +23415,7 @@
         <v>-2.70235217998757</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>0.12195122</v>
       </c>
@@ -23404,7 +23423,7 @@
         <v>-1.6990500711237899</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>0.12195122</v>
       </c>

</xml_diff>